<commit_message>
Implemented Nsp3 domain classifier into weekly update pipeline
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="677">
   <si>
     <t>PDB</t>
   </si>
@@ -1848,6 +1848,15 @@
     <t>STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH 4- (2-HYDROXYETHYL)PHENOL</t>
   </si>
   <si>
+    <t>7sgu</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER608 INHIBITOR</t>
+  </si>
+  <si>
+    <t>2021-10-07</t>
+  </si>
+  <si>
     <t>7rbr</t>
   </si>
   <si>
@@ -1947,6 +1956,12 @@
     <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER530 INHIBITOR</t>
   </si>
   <si>
+    <t>7sgw</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER630 INHIBITOR</t>
+  </si>
+  <si>
     <t>7rzc</t>
   </si>
   <si>
@@ -1972,6 +1987,12 @@
   </si>
   <si>
     <t>2020-06-16</t>
+  </si>
+  <si>
+    <t>7sgv</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER630 INHIBITOR</t>
   </si>
   <si>
     <t>7lbs</t>
@@ -6900,7 +6921,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7273,7 +7294,7 @@
         <v>609</v>
       </c>
       <c r="B22">
-        <v>1.88</v>
+        <v>1.79</v>
       </c>
       <c r="C22" t="s">
         <v>610</v>
@@ -7282,24 +7303,24 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>586</v>
+        <v>611</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B23">
-        <v>1.6</v>
+        <v>1.88</v>
       </c>
       <c r="C23" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>613</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -7307,7 +7328,7 @@
         <v>614</v>
       </c>
       <c r="B24">
-        <v>2.9</v>
+        <v>1.6</v>
       </c>
       <c r="C24" t="s">
         <v>615</v>
@@ -7324,7 +7345,7 @@
         <v>617</v>
       </c>
       <c r="B25">
-        <v>1.95</v>
+        <v>2.9</v>
       </c>
       <c r="C25" t="s">
         <v>618</v>
@@ -7333,24 +7354,24 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>568</v>
+        <v>619</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B26">
-        <v>2.9</v>
+        <v>1.95</v>
       </c>
       <c r="C26" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>621</v>
+        <v>568</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7358,7 +7379,7 @@
         <v>622</v>
       </c>
       <c r="B27">
-        <v>2.48</v>
+        <v>2.9</v>
       </c>
       <c r="C27" t="s">
         <v>623</v>
@@ -7375,7 +7396,7 @@
         <v>625</v>
       </c>
       <c r="B28">
-        <v>3.2</v>
+        <v>2.48</v>
       </c>
       <c r="C28" t="s">
         <v>626</v>
@@ -7392,7 +7413,7 @@
         <v>628</v>
       </c>
       <c r="B29">
-        <v>1.93</v>
+        <v>3.2</v>
       </c>
       <c r="C29" t="s">
         <v>629</v>
@@ -7409,7 +7430,7 @@
         <v>631</v>
       </c>
       <c r="B30">
-        <v>2.72</v>
+        <v>1.93</v>
       </c>
       <c r="C30" t="s">
         <v>632</v>
@@ -7426,7 +7447,7 @@
         <v>634</v>
       </c>
       <c r="B31">
-        <v>1.97</v>
+        <v>2.72</v>
       </c>
       <c r="C31" t="s">
         <v>635</v>
@@ -7443,7 +7464,7 @@
         <v>637</v>
       </c>
       <c r="B32">
-        <v>2.3</v>
+        <v>1.97</v>
       </c>
       <c r="C32" t="s">
         <v>638</v>
@@ -7469,24 +7490,24 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>568</v>
+        <v>642</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B34">
-        <v>2.04</v>
+        <v>2.3</v>
       </c>
       <c r="C34" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>644</v>
+        <v>568</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -7494,7 +7515,7 @@
         <v>645</v>
       </c>
       <c r="B35">
-        <v>1.66</v>
+        <v>1.95</v>
       </c>
       <c r="C35" t="s">
         <v>646</v>
@@ -7503,41 +7524,41 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
+        <v>647</v>
+      </c>
+      <c r="B36">
+        <v>2.04</v>
+      </c>
+      <c r="C36" t="s">
         <v>648</v>
       </c>
-      <c r="B36">
-        <v>2.48</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
         <v>649</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
+        <v>650</v>
+      </c>
+      <c r="B37">
+        <v>1.66</v>
+      </c>
+      <c r="C37" t="s">
         <v>651</v>
       </c>
-      <c r="B37">
-        <v>2.8</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
         <v>652</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -7545,7 +7566,7 @@
         <v>653</v>
       </c>
       <c r="B38">
-        <v>2.5</v>
+        <v>2.48</v>
       </c>
       <c r="C38" t="s">
         <v>654</v>
@@ -7562,7 +7583,7 @@
         <v>656</v>
       </c>
       <c r="B39">
-        <v>2.02</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
         <v>657</v>
@@ -7571,7 +7592,7 @@
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>562</v>
+        <v>611</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -7579,7 +7600,7 @@
         <v>658</v>
       </c>
       <c r="B40">
-        <v>2.05</v>
+        <v>2.8</v>
       </c>
       <c r="C40" t="s">
         <v>659</v>
@@ -7588,6 +7609,57 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>660</v>
+      </c>
+      <c r="B41">
+        <v>2.5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>661</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>663</v>
+      </c>
+      <c r="B42">
+        <v>2.02</v>
+      </c>
+      <c r="C42" t="s">
+        <v>664</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>665</v>
+      </c>
+      <c r="B43">
+        <v>2.05</v>
+      </c>
+      <c r="C43" t="s">
+        <v>666</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
         <v>568</v>
       </c>
     </row>
@@ -7628,7 +7700,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>660</v>
+        <v>667</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -7645,7 +7717,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -7697,19 +7769,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="B2">
         <v>2.45</v>
       </c>
       <c r="C2" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -7749,19 +7821,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>665</v>
+        <v>672</v>
       </c>
       <c r="B2">
         <v>2.17</v>
       </c>
       <c r="C2" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
     </row>
   </sheetData>
@@ -7801,19 +7873,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>668</v>
+        <v>675</v>
       </c>
       <c r="B2">
         <v>3.21</v>
       </c>
       <c r="C2" t="s">
-        <v>669</v>
+        <v>676</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified sequences for domain classifier
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
@@ -10,9 +10,9 @@
     <sheet name="nsp3_Macro1" sheetId="1" r:id="rId1"/>
     <sheet name="nsp3_PL2pro" sheetId="2" r:id="rId2"/>
     <sheet name="nsp3_NAB" sheetId="3" r:id="rId3"/>
-    <sheet name="CoV1_nsp3_LINKER-PLpro-NAB" sheetId="4" r:id="rId4"/>
-    <sheet name="nsp3_Y3" sheetId="5" r:id="rId5"/>
-    <sheet name="nsp3_frgmnt_btwn_PL2pro_NAB" sheetId="6" r:id="rId6"/>
+    <sheet name="nsp3_Ubl2" sheetId="4" r:id="rId4"/>
+    <sheet name="nsp3_LINKER-PLpro-NAB" sheetId="5" r:id="rId5"/>
+    <sheet name="nsp3_Y3" sheetId="6" r:id="rId6"/>
     <sheet name="nsp3_Ubl1" sheetId="7" r:id="rId7"/>
     <sheet name="Organisms" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -1733,6 +1733,285 @@
     <t>2020-07-27</t>
   </si>
   <si>
+    <t>7d7k</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE IN APO FORM</t>
+  </si>
+  <si>
+    <t>2020-10-04</t>
+  </si>
+  <si>
+    <t>7lbr</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-89</t>
+  </si>
+  <si>
+    <t>2021-01-08</t>
+  </si>
+  <si>
+    <t>6wuu</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE SARS COV-2 PAPAIN-LIKE PROTEASE IN COMPLEX WITH PEPTIDE INHIBITOR VIR250</t>
+  </si>
+  <si>
+    <t>2020-05-05</t>
+  </si>
+  <si>
+    <t>7rbs</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH HUMAN ISG15</t>
+  </si>
+  <si>
+    <t>2021-07-06</t>
+  </si>
+  <si>
+    <t>7oft</t>
+  </si>
+  <si>
+    <t>STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH P- HYDROXYBENZALDEHYDE</t>
+  </si>
+  <si>
+    <t>2021-05-05</t>
+  </si>
+  <si>
+    <t>6wzu</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , P3221 SPACE GROUP</t>
+  </si>
+  <si>
+    <t>2020-05-14</t>
+  </si>
+  <si>
+    <t>7d7l</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE IN COMPLEX WITH YM155</t>
+  </si>
+  <si>
+    <t>6xaa</t>
+  </si>
+  <si>
+    <t>SARS COV-2 PLPRO IN COMPLEX WITH UBIQUITIN PROPARGYLAMIDE</t>
+  </si>
+  <si>
+    <t>2020-06-04</t>
+  </si>
+  <si>
+    <t>6wrh</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT</t>
+  </si>
+  <si>
+    <t>7e35</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) C112S MUTANT BOUND TO COMPOUND S43</t>
+  </si>
+  <si>
+    <t>2021-02-08</t>
+  </si>
+  <si>
+    <t>6xa9</t>
+  </si>
+  <si>
+    <t>SARS COV-2 PLPRO IN COMPLEX WITH ISG15 C-TERMINAL DOMAIN PROPARGYLAMIDE</t>
+  </si>
+  <si>
+    <t>7kol</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER496 INHIBITOR</t>
+  </si>
+  <si>
+    <t>7ofs</t>
+  </si>
+  <si>
+    <t>STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH 4- (2-HYDROXYETHYL)PHENOL</t>
+  </si>
+  <si>
+    <t>7sgu</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER608 INHIBITOR</t>
+  </si>
+  <si>
+    <t>2021-10-07</t>
+  </si>
+  <si>
+    <t>7rbr</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH A LYS48-LINKED DI-UBIQUITIN</t>
+  </si>
+  <si>
+    <t>7d6h</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) C112S MUTANT</t>
+  </si>
+  <si>
+    <t>2020-09-30</t>
+  </si>
+  <si>
+    <t>7llz</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-69</t>
+  </si>
+  <si>
+    <t>2021-02-04</t>
+  </si>
+  <si>
+    <t>7jit</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT, IN COMPLEX WITH PLP_SNYDER495 INHIBITOR</t>
+  </si>
+  <si>
+    <t>7los</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-65</t>
+  </si>
+  <si>
+    <t>2021-02-10</t>
+  </si>
+  <si>
+    <t>7jrn</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE WILD TYPE SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) WITH INHIBITOR GRL0617</t>
+  </si>
+  <si>
+    <t>2020-08-12</t>
+  </si>
+  <si>
+    <t>7cjm</t>
+  </si>
+  <si>
+    <t>SARS COV-2 PLPRO IN COMPLEX WITH GRL0617</t>
+  </si>
+  <si>
+    <t>2020-07-11</t>
+  </si>
+  <si>
+    <t>7jn2</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER441 INHIBITOR</t>
+  </si>
+  <si>
+    <t>2020-08-03</t>
+  </si>
+  <si>
+    <t>7krx</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER441 INHIBITOR</t>
+  </si>
+  <si>
+    <t>2020-11-20</t>
+  </si>
+  <si>
+    <t>7d47</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE C111S</t>
+  </si>
+  <si>
+    <t>2020-09-22</t>
+  </si>
+  <si>
+    <t>7llf</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-83</t>
+  </si>
+  <si>
+    <t>2021-02-03</t>
+  </si>
+  <si>
+    <t>7sgw</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER630 INHIBITOR</t>
+  </si>
+  <si>
+    <t>7rzc</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH JUN9-84-3 INHIBITOR</t>
+  </si>
+  <si>
+    <t>2021-08-27</t>
+  </si>
+  <si>
+    <t>6wx4</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE SARS COV-2 PAPAIN-LIKE PROTEASE IN COMPLEX WITH PEPTIDE INHIBITOR VIR251</t>
+  </si>
+  <si>
+    <t>2020-05-09</t>
+  </si>
+  <si>
+    <t>6xg3</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT, AT ROOM TEMPERATURE</t>
+  </si>
+  <si>
+    <t>2020-06-16</t>
+  </si>
+  <si>
+    <t>7sgv</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER630 INHIBITOR</t>
+  </si>
+  <si>
+    <t>7lbs</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-24</t>
+  </si>
+  <si>
+    <t>7cjd</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE SARS-COV-2 PLPRO C111S MUTANT</t>
+  </si>
+  <si>
+    <t>2020-07-10</t>
+  </si>
+  <si>
+    <t>7koj</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER494 INHIBITOR</t>
+  </si>
+  <si>
+    <t>7jiv</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT, IN COMPLEX WITH PLP_SNYDER530 INHIBITOR</t>
+  </si>
+  <si>
+    <t>7lgo</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE NUCLEIC ACID BINDING DOMAIN (NAB) OF NSP3 FROM SARS-COV-2</t>
+  </si>
+  <si>
+    <t>2021-01-20</t>
+  </si>
+  <si>
     <t>6yva</t>
   </si>
   <si>
@@ -1742,291 +2021,18 @@
     <t>2020-04-28</t>
   </si>
   <si>
-    <t>7d7k</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE IN APO FORM</t>
-  </si>
-  <si>
-    <t>2020-10-04</t>
-  </si>
-  <si>
-    <t>7lbr</t>
-  </si>
-  <si>
-    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-89</t>
-  </si>
-  <si>
-    <t>2021-01-08</t>
-  </si>
-  <si>
-    <t>6wuu</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF THE SARS COV-2 PAPAIN-LIKE PROTEASE IN COMPLEX WITH PEPTIDE INHIBITOR VIR250</t>
-  </si>
-  <si>
-    <t>2020-05-05</t>
-  </si>
-  <si>
-    <t>7rbs</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH HUMAN ISG15</t>
-  </si>
-  <si>
-    <t>2021-07-06</t>
-  </si>
-  <si>
-    <t>7oft</t>
-  </si>
-  <si>
-    <t>STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH P- HYDROXYBENZALDEHYDE</t>
-  </si>
-  <si>
-    <t>2021-05-05</t>
-  </si>
-  <si>
-    <t>6wzu</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , P3221 SPACE GROUP</t>
-  </si>
-  <si>
-    <t>2020-05-14</t>
-  </si>
-  <si>
-    <t>7d7l</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE IN COMPLEX WITH YM155</t>
-  </si>
-  <si>
-    <t>6xaa</t>
-  </si>
-  <si>
-    <t>SARS COV-2 PLPRO IN COMPLEX WITH UBIQUITIN PROPARGYLAMIDE</t>
-  </si>
-  <si>
-    <t>2020-06-04</t>
-  </si>
-  <si>
-    <t>6wrh</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT</t>
-  </si>
-  <si>
-    <t>7e35</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF THE SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) C112S MUTANT BOUND TO COMPOUND S43</t>
-  </si>
-  <si>
-    <t>2021-02-08</t>
-  </si>
-  <si>
-    <t>6xa9</t>
-  </si>
-  <si>
-    <t>SARS COV-2 PLPRO IN COMPLEX WITH ISG15 C-TERMINAL DOMAIN PROPARGYLAMIDE</t>
-  </si>
-  <si>
-    <t>7kol</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER496 INHIBITOR</t>
-  </si>
-  <si>
-    <t>7ofs</t>
-  </si>
-  <si>
-    <t>STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH 4- (2-HYDROXYETHYL)PHENOL</t>
-  </si>
-  <si>
-    <t>7sgu</t>
-  </si>
-  <si>
-    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER608 INHIBITOR</t>
-  </si>
-  <si>
-    <t>2021-10-07</t>
-  </si>
-  <si>
-    <t>7rbr</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH A LYS48-LINKED DI-UBIQUITIN</t>
-  </si>
-  <si>
-    <t>7d6h</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF THE SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) C112S MUTANT</t>
-  </si>
-  <si>
-    <t>2020-09-30</t>
-  </si>
-  <si>
-    <t>7llz</t>
-  </si>
-  <si>
-    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-69</t>
-  </si>
-  <si>
-    <t>2021-02-04</t>
-  </si>
-  <si>
-    <t>7jit</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT, IN COMPLEX WITH PLP_SNYDER495 INHIBITOR</t>
-  </si>
-  <si>
-    <t>7los</t>
-  </si>
-  <si>
-    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-65</t>
-  </si>
-  <si>
-    <t>2021-02-10</t>
-  </si>
-  <si>
-    <t>7jrn</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF THE WILD TYPE SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) WITH INHIBITOR GRL0617</t>
-  </si>
-  <si>
-    <t>2020-08-12</t>
-  </si>
-  <si>
-    <t>7cjm</t>
-  </si>
-  <si>
-    <t>SARS COV-2 PLPRO IN COMPLEX WITH GRL0617</t>
-  </si>
-  <si>
-    <t>2020-07-11</t>
-  </si>
-  <si>
-    <t>7jn2</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER441 INHIBITOR</t>
-  </si>
-  <si>
-    <t>2020-08-03</t>
-  </si>
-  <si>
-    <t>7krx</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER441 INHIBITOR</t>
-  </si>
-  <si>
-    <t>2020-11-20</t>
-  </si>
-  <si>
-    <t>7d47</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE C111S</t>
-  </si>
-  <si>
-    <t>2020-09-22</t>
-  </si>
-  <si>
-    <t>7llf</t>
-  </si>
-  <si>
-    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-83</t>
-  </si>
-  <si>
-    <t>2021-02-03</t>
-  </si>
-  <si>
-    <t>7sgw</t>
-  </si>
-  <si>
-    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER630 INHIBITOR</t>
-  </si>
-  <si>
-    <t>7rzc</t>
-  </si>
-  <si>
-    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH JUN9-84-3 INHIBITOR</t>
-  </si>
-  <si>
-    <t>2021-08-27</t>
-  </si>
-  <si>
-    <t>6wx4</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF THE SARS COV-2 PAPAIN-LIKE PROTEASE IN COMPLEX WITH PEPTIDE INHIBITOR VIR251</t>
-  </si>
-  <si>
-    <t>2020-05-09</t>
-  </si>
-  <si>
-    <t>6xg3</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT, AT ROOM TEMPERATURE</t>
-  </si>
-  <si>
-    <t>2020-06-16</t>
-  </si>
-  <si>
-    <t>7sgv</t>
-  </si>
-  <si>
-    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER630 INHIBITOR</t>
-  </si>
-  <si>
-    <t>7lbs</t>
-  </si>
-  <si>
-    <t>SARS-COV-2 PAPAIN-LIKE PROTEASE (PLPRO) BOUND TO INHIBITOR XR8-24</t>
-  </si>
-  <si>
-    <t>7cjd</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF THE SARS-COV-2 PLPRO C111S MUTANT</t>
-  </si>
-  <si>
-    <t>2020-07-10</t>
-  </si>
-  <si>
-    <t>7koj</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH PLP_SNYDER494 INHIBITOR</t>
-  </si>
-  <si>
-    <t>7jiv</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT, IN COMPLEX WITH PLP_SNYDER530 INHIBITOR</t>
-  </si>
-  <si>
-    <t>7lgo</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF THE NUCLEIC ACID BINDING DOMAIN (NAB) OF NSP3 FROM SARS-COV-2</t>
-  </si>
-  <si>
-    <t>2021-01-20</t>
-  </si>
-  <si>
     <t>7kqw</t>
   </si>
   <si>
     <t>CRYSTAL STRUCTURE OF SARS-COV-2 NSP3 MACRODOMAIN (C2 CRYSTAL FORM, METHYLATED)</t>
   </si>
   <si>
+    <t>7jiw</t>
+  </si>
+  <si>
+    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER530 INHIBITOR</t>
+  </si>
+  <si>
     <t>7rqg</t>
   </si>
   <si>
@@ -2034,12 +2040,6 @@
   </si>
   <si>
     <t>2021-08-06</t>
-  </si>
-  <si>
-    <t>7jiw</t>
-  </si>
-  <si>
-    <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 IN COMPLEX WITH PLP_SNYDER530 INHIBITOR</t>
   </si>
   <si>
     <t>7kag</t>
@@ -6918,7 +6918,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7053,7 +7053,7 @@
         <v>570</v>
       </c>
       <c r="B8">
-        <v>3.18</v>
+        <v>1.9</v>
       </c>
       <c r="C8" t="s">
         <v>571</v>
@@ -7070,7 +7070,7 @@
         <v>573</v>
       </c>
       <c r="B9">
-        <v>1.9</v>
+        <v>2.2</v>
       </c>
       <c r="C9" t="s">
         <v>574</v>
@@ -7087,7 +7087,7 @@
         <v>576</v>
       </c>
       <c r="B10">
-        <v>2.2</v>
+        <v>2.79</v>
       </c>
       <c r="C10" t="s">
         <v>577</v>
@@ -7104,7 +7104,7 @@
         <v>579</v>
       </c>
       <c r="B11">
-        <v>2.79</v>
+        <v>2.98</v>
       </c>
       <c r="C11" t="s">
         <v>580</v>
@@ -7121,7 +7121,7 @@
         <v>582</v>
       </c>
       <c r="B12">
-        <v>2.98</v>
+        <v>1.95</v>
       </c>
       <c r="C12" t="s">
         <v>583</v>
@@ -7138,7 +7138,7 @@
         <v>585</v>
       </c>
       <c r="B13">
-        <v>1.95</v>
+        <v>1.79</v>
       </c>
       <c r="C13" t="s">
         <v>586</v>
@@ -7155,7 +7155,7 @@
         <v>588</v>
       </c>
       <c r="B14">
-        <v>1.79</v>
+        <v>2.11</v>
       </c>
       <c r="C14" t="s">
         <v>589</v>
@@ -7164,24 +7164,24 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>590</v>
+      </c>
+      <c r="B15">
+        <v>2.7</v>
+      </c>
+      <c r="C15" t="s">
         <v>591</v>
       </c>
-      <c r="B15">
-        <v>2.11</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>592</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7189,7 +7189,7 @@
         <v>593</v>
       </c>
       <c r="B16">
-        <v>2.7</v>
+        <v>1.6</v>
       </c>
       <c r="C16" t="s">
         <v>594</v>
@@ -7198,24 +7198,24 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>595</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>595</v>
+      </c>
+      <c r="B17">
+        <v>2.4</v>
+      </c>
+      <c r="C17" t="s">
         <v>596</v>
       </c>
-      <c r="B17">
-        <v>1.6</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
         <v>597</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7223,7 +7223,7 @@
         <v>598</v>
       </c>
       <c r="B18">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="C18" t="s">
         <v>599</v>
@@ -7232,58 +7232,58 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
+        <v>600</v>
+      </c>
+      <c r="B19">
+        <v>2.58</v>
+      </c>
+      <c r="C19" t="s">
         <v>601</v>
       </c>
-      <c r="B19">
-        <v>2.9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>602</v>
-      </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>595</v>
+        <v>560</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
+        <v>602</v>
+      </c>
+      <c r="B20">
+        <v>1.9</v>
+      </c>
+      <c r="C20" t="s">
         <v>603</v>
       </c>
-      <c r="B20">
-        <v>2.58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>604</v>
-      </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>560</v>
+        <v>584</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
+        <v>604</v>
+      </c>
+      <c r="B21">
+        <v>1.79</v>
+      </c>
+      <c r="C21" t="s">
         <v>605</v>
       </c>
-      <c r="B21">
-        <v>1.9</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
         <v>606</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -7291,7 +7291,7 @@
         <v>607</v>
       </c>
       <c r="B22">
-        <v>1.79</v>
+        <v>1.88</v>
       </c>
       <c r="C22" t="s">
         <v>608</v>
@@ -7300,24 +7300,24 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>609</v>
+        <v>581</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
+        <v>609</v>
+      </c>
+      <c r="B23">
+        <v>1.6</v>
+      </c>
+      <c r="C23" t="s">
         <v>610</v>
       </c>
-      <c r="B23">
-        <v>1.88</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
         <v>611</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -7325,7 +7325,7 @@
         <v>612</v>
       </c>
       <c r="B24">
-        <v>1.6</v>
+        <v>2.9</v>
       </c>
       <c r="C24" t="s">
         <v>613</v>
@@ -7342,7 +7342,7 @@
         <v>615</v>
       </c>
       <c r="B25">
-        <v>2.9</v>
+        <v>1.95</v>
       </c>
       <c r="C25" t="s">
         <v>616</v>
@@ -7351,24 +7351,24 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>617</v>
+        <v>566</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
+        <v>617</v>
+      </c>
+      <c r="B26">
+        <v>2.9</v>
+      </c>
+      <c r="C26" t="s">
         <v>618</v>
       </c>
-      <c r="B26">
-        <v>1.95</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
         <v>619</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7376,7 +7376,7 @@
         <v>620</v>
       </c>
       <c r="B27">
-        <v>2.9</v>
+        <v>2.48</v>
       </c>
       <c r="C27" t="s">
         <v>621</v>
@@ -7393,7 +7393,7 @@
         <v>623</v>
       </c>
       <c r="B28">
-        <v>2.48</v>
+        <v>3.2</v>
       </c>
       <c r="C28" t="s">
         <v>624</v>
@@ -7410,7 +7410,7 @@
         <v>626</v>
       </c>
       <c r="B29">
-        <v>3.2</v>
+        <v>1.93</v>
       </c>
       <c r="C29" t="s">
         <v>627</v>
@@ -7427,7 +7427,7 @@
         <v>629</v>
       </c>
       <c r="B30">
-        <v>1.93</v>
+        <v>2.72</v>
       </c>
       <c r="C30" t="s">
         <v>630</v>
@@ -7444,7 +7444,7 @@
         <v>632</v>
       </c>
       <c r="B31">
-        <v>2.72</v>
+        <v>1.97</v>
       </c>
       <c r="C31" t="s">
         <v>633</v>
@@ -7461,7 +7461,7 @@
         <v>635</v>
       </c>
       <c r="B32">
-        <v>1.97</v>
+        <v>2.3</v>
       </c>
       <c r="C32" t="s">
         <v>636</v>
@@ -7478,7 +7478,7 @@
         <v>638</v>
       </c>
       <c r="B33">
-        <v>2.3</v>
+        <v>1.95</v>
       </c>
       <c r="C33" t="s">
         <v>639</v>
@@ -7487,24 +7487,24 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>640</v>
+        <v>606</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
+        <v>640</v>
+      </c>
+      <c r="B34">
+        <v>2.04</v>
+      </c>
+      <c r="C34" t="s">
         <v>641</v>
       </c>
-      <c r="B34">
-        <v>1.95</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
         <v>642</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -7512,7 +7512,7 @@
         <v>643</v>
       </c>
       <c r="B35">
-        <v>2.04</v>
+        <v>1.66</v>
       </c>
       <c r="C35" t="s">
         <v>644</v>
@@ -7529,7 +7529,7 @@
         <v>646</v>
       </c>
       <c r="B36">
-        <v>1.66</v>
+        <v>2.48</v>
       </c>
       <c r="C36" t="s">
         <v>647</v>
@@ -7546,7 +7546,7 @@
         <v>649</v>
       </c>
       <c r="B37">
-        <v>2.48</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>650</v>
@@ -7555,41 +7555,41 @@
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>651</v>
+        <v>606</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
+        <v>651</v>
+      </c>
+      <c r="B38">
+        <v>2.8</v>
+      </c>
+      <c r="C38" t="s">
         <v>652</v>
       </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>653</v>
-      </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>609</v>
+        <v>575</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
+        <v>653</v>
+      </c>
+      <c r="B39">
+        <v>2.5</v>
+      </c>
+      <c r="C39" t="s">
         <v>654</v>
       </c>
-      <c r="B39">
-        <v>2.8</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
         <v>655</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -7597,7 +7597,7 @@
         <v>656</v>
       </c>
       <c r="B40">
-        <v>2.5</v>
+        <v>2.02</v>
       </c>
       <c r="C40" t="s">
         <v>657</v>
@@ -7606,40 +7606,23 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>658</v>
+        <v>560</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
+        <v>658</v>
+      </c>
+      <c r="B41">
+        <v>2.05</v>
+      </c>
+      <c r="C41" t="s">
         <v>659</v>
       </c>
-      <c r="B41">
-        <v>2.02</v>
-      </c>
-      <c r="C41" t="s">
-        <v>660</v>
-      </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>661</v>
-      </c>
-      <c r="B42">
-        <v>2.05</v>
-      </c>
-      <c r="C42" t="s">
-        <v>662</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" t="s">
         <v>566</v>
       </c>
     </row>
@@ -7680,19 +7663,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B2">
         <v>2.45</v>
       </c>
       <c r="C2" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
   </sheetData>
@@ -7732,19 +7715,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B2">
-        <v>0.93</v>
+        <v>3.18</v>
       </c>
       <c r="C2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>413</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>
@@ -7754,7 +7737,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7784,19 +7767,36 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>666</v>
+      </c>
+      <c r="B2">
+        <v>0.93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>668</v>
       </c>
-      <c r="B2">
-        <v>2.17</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3">
+        <v>2.3</v>
+      </c>
+      <c r="C3" t="s">
         <v>669</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>670</v>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -7836,19 +7836,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B2">
+        <v>2.17</v>
+      </c>
+      <c r="C2" t="s">
         <v>671</v>
       </c>
-      <c r="B2">
-        <v>2.3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>672</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>566</v>
       </c>
     </row>
   </sheetData>
@@ -7900,7 +7900,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="43" spans="2:2">
@@ -8167,7 +8167,7 @@
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>570</v>
+        <v>663</v>
       </c>
     </row>
     <row r="50" spans="2:2">
@@ -8182,7 +8182,7 @@
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="53" spans="2:2">
@@ -8252,7 +8252,7 @@
     </row>
     <row r="66" spans="2:2">
       <c r="B66" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="67" spans="2:2">
@@ -8272,7 +8272,7 @@
     </row>
     <row r="70" spans="2:2">
       <c r="B70" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="71" spans="2:2">
@@ -8292,7 +8292,7 @@
     </row>
     <row r="74" spans="2:2">
       <c r="B74" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="75" spans="2:2">
@@ -8337,7 +8337,7 @@
     </row>
     <row r="83" spans="2:2">
       <c r="B83" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="84" spans="2:2">
@@ -8372,7 +8372,7 @@
     </row>
     <row r="90" spans="2:2">
       <c r="B90" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="91" spans="2:2">
@@ -8392,7 +8392,7 @@
     </row>
     <row r="94" spans="2:2">
       <c r="B94" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="95" spans="2:2">
@@ -8512,7 +8512,7 @@
     </row>
     <row r="118" spans="2:2">
       <c r="B118" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="119" spans="2:2">
@@ -8562,7 +8562,7 @@
     </row>
     <row r="128" spans="2:2">
       <c r="B128" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="129" spans="2:2">
@@ -8572,7 +8572,7 @@
     </row>
     <row r="130" spans="2:2">
       <c r="B130" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="131" spans="2:2">
@@ -8597,7 +8597,7 @@
     </row>
     <row r="135" spans="2:2">
       <c r="B135" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="136" spans="2:2">
@@ -8612,7 +8612,7 @@
     </row>
     <row r="138" spans="2:2">
       <c r="B138" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="139" spans="2:2">
@@ -8652,7 +8652,7 @@
     </row>
     <row r="146" spans="2:2">
       <c r="B146" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="147" spans="2:2">
@@ -8707,7 +8707,7 @@
     </row>
     <row r="157" spans="2:2">
       <c r="B157" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="158" spans="2:2">
@@ -8727,7 +8727,7 @@
     </row>
     <row r="161" spans="2:2">
       <c r="B161" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="162" spans="2:2">
@@ -8757,7 +8757,7 @@
     </row>
     <row r="167" spans="2:2">
       <c r="B167" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="168" spans="2:2">
@@ -8772,7 +8772,7 @@
     </row>
     <row r="170" spans="2:2">
       <c r="B170" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="171" spans="2:2">
@@ -8787,7 +8787,7 @@
     </row>
     <row r="173" spans="2:2">
       <c r="B173" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="174" spans="2:2">
@@ -8797,7 +8797,7 @@
     </row>
     <row r="175" spans="2:2">
       <c r="B175" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="176" spans="2:2">
@@ -8857,7 +8857,7 @@
     </row>
     <row r="187" spans="2:2">
       <c r="B187" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="188" spans="2:2">
@@ -8897,12 +8897,12 @@
     </row>
     <row r="195" spans="2:2">
       <c r="B195" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="197" spans="2:2">
@@ -8922,7 +8922,7 @@
     </row>
     <row r="200" spans="2:2">
       <c r="B200" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="201" spans="2:2">
@@ -8932,7 +8932,7 @@
     </row>
     <row r="202" spans="2:2">
       <c r="B202" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="203" spans="2:2">
@@ -8982,12 +8982,12 @@
     </row>
     <row r="212" spans="2:2">
       <c r="B212" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="213" spans="2:2">
       <c r="B213" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="214" spans="2:2">
@@ -9037,7 +9037,7 @@
     </row>
     <row r="223" spans="2:2">
       <c r="B223" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="224" spans="2:2">
@@ -9067,7 +9067,7 @@
     </row>
     <row r="229" spans="2:2">
       <c r="B229" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="230" spans="2:2">
@@ -9122,7 +9122,7 @@
     </row>
     <row r="240" spans="2:2">
       <c r="B240" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="241" spans="2:2">
@@ -9147,7 +9147,7 @@
     </row>
     <row r="245" spans="2:2">
       <c r="B245" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="246" spans="2:2">
@@ -9252,7 +9252,7 @@
     </row>
     <row r="266" spans="2:2">
       <c r="B266" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="267" spans="2:2">
@@ -9277,7 +9277,7 @@
     </row>
     <row r="271" spans="2:2">
       <c r="B271" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="272" spans="2:2">
@@ -9387,17 +9387,17 @@
     </row>
     <row r="293" spans="2:2">
       <c r="B293" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="296" spans="2:2">
@@ -9437,7 +9437,7 @@
     </row>
     <row r="303" spans="2:2">
       <c r="B303" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="304" spans="2:2">
@@ -9490,7 +9490,7 @@
         <v>678</v>
       </c>
       <c r="B314" t="s">
-        <v>570</v>
+        <v>663</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -9498,12 +9498,12 @@
         <v>679</v>
       </c>
       <c r="B316" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="317" spans="1:2">
       <c r="B317" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -9511,22 +9511,22 @@
         <v>680</v>
       </c>
       <c r="B319" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="320" spans="1:2">
       <c r="B320" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="321" spans="2:2">
       <c r="B321" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="322" spans="2:2">
       <c r="B322" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weekly update, 2021-11-17, SARS-CoV-2
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
@@ -11,7 +11,7 @@
     <sheet name="nsp3_PL2pro" sheetId="2" r:id="rId2"/>
     <sheet name="nsp3_NAB" sheetId="3" r:id="rId3"/>
     <sheet name="nsp3_Ubl2" sheetId="4" r:id="rId4"/>
-    <sheet name="nsp3_LINKER-PLpro-NAB" sheetId="5" r:id="rId5"/>
+    <sheet name="nsp3_pred_linker-Ecto-TM2" sheetId="5" r:id="rId5"/>
     <sheet name="nsp3_Y3" sheetId="6" r:id="rId6"/>
     <sheet name="nsp3_Ubl1" sheetId="7" r:id="rId7"/>
     <sheet name="Organisms" sheetId="8" r:id="rId8"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="684">
   <si>
     <t>PDB</t>
   </si>
@@ -1833,6 +1833,15 @@
   </si>
   <si>
     <t>STRUCTURE OF SARS-COV-2 PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH 4- (2-HYDROXYETHYL)PHENOL</t>
+  </si>
+  <si>
+    <t>7sqe</t>
+  </si>
+  <si>
+    <t>PAPAIN-LIKE PROTEASE OF SARS COV-2, C111S MUTANT, IN COMPLEX WITH JUN9-84-3 INHIBITOR</t>
+  </si>
+  <si>
+    <t>2021-11-05</t>
   </si>
   <si>
     <t>7sgu</t>
@@ -6918,7 +6927,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7274,7 +7283,7 @@
         <v>604</v>
       </c>
       <c r="B21">
-        <v>1.79</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>605</v>
@@ -7291,7 +7300,7 @@
         <v>607</v>
       </c>
       <c r="B22">
-        <v>1.88</v>
+        <v>1.79</v>
       </c>
       <c r="C22" t="s">
         <v>608</v>
@@ -7300,24 +7309,24 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>581</v>
+        <v>609</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B23">
-        <v>1.6</v>
+        <v>1.88</v>
       </c>
       <c r="C23" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>611</v>
+        <v>581</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -7325,7 +7334,7 @@
         <v>612</v>
       </c>
       <c r="B24">
-        <v>2.9</v>
+        <v>1.6</v>
       </c>
       <c r="C24" t="s">
         <v>613</v>
@@ -7342,7 +7351,7 @@
         <v>615</v>
       </c>
       <c r="B25">
-        <v>1.95</v>
+        <v>2.9</v>
       </c>
       <c r="C25" t="s">
         <v>616</v>
@@ -7351,24 +7360,24 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>566</v>
+        <v>617</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B26">
-        <v>2.9</v>
+        <v>1.95</v>
       </c>
       <c r="C26" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>619</v>
+        <v>566</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7376,7 +7385,7 @@
         <v>620</v>
       </c>
       <c r="B27">
-        <v>2.48</v>
+        <v>2.9</v>
       </c>
       <c r="C27" t="s">
         <v>621</v>
@@ -7393,7 +7402,7 @@
         <v>623</v>
       </c>
       <c r="B28">
-        <v>3.2</v>
+        <v>2.48</v>
       </c>
       <c r="C28" t="s">
         <v>624</v>
@@ -7410,7 +7419,7 @@
         <v>626</v>
       </c>
       <c r="B29">
-        <v>1.93</v>
+        <v>3.2</v>
       </c>
       <c r="C29" t="s">
         <v>627</v>
@@ -7427,7 +7436,7 @@
         <v>629</v>
       </c>
       <c r="B30">
-        <v>2.72</v>
+        <v>1.93</v>
       </c>
       <c r="C30" t="s">
         <v>630</v>
@@ -7444,7 +7453,7 @@
         <v>632</v>
       </c>
       <c r="B31">
-        <v>1.97</v>
+        <v>2.72</v>
       </c>
       <c r="C31" t="s">
         <v>633</v>
@@ -7461,7 +7470,7 @@
         <v>635</v>
       </c>
       <c r="B32">
-        <v>2.3</v>
+        <v>1.97</v>
       </c>
       <c r="C32" t="s">
         <v>636</v>
@@ -7478,7 +7487,7 @@
         <v>638</v>
       </c>
       <c r="B33">
-        <v>1.95</v>
+        <v>2.3</v>
       </c>
       <c r="C33" t="s">
         <v>639</v>
@@ -7487,24 +7496,24 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>606</v>
+        <v>640</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B34">
-        <v>2.04</v>
+        <v>1.95</v>
       </c>
       <c r="C34" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>642</v>
+        <v>609</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -7512,7 +7521,7 @@
         <v>643</v>
       </c>
       <c r="B35">
-        <v>1.66</v>
+        <v>2.04</v>
       </c>
       <c r="C35" t="s">
         <v>644</v>
@@ -7529,7 +7538,7 @@
         <v>646</v>
       </c>
       <c r="B36">
-        <v>2.48</v>
+        <v>1.66</v>
       </c>
       <c r="C36" t="s">
         <v>647</v>
@@ -7546,7 +7555,7 @@
         <v>649</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>2.48</v>
       </c>
       <c r="C37" t="s">
         <v>650</v>
@@ -7555,41 +7564,41 @@
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>606</v>
+        <v>651</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B38">
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B39">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="C39" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>655</v>
+        <v>575</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -7597,7 +7606,7 @@
         <v>656</v>
       </c>
       <c r="B40">
-        <v>2.02</v>
+        <v>2.5</v>
       </c>
       <c r="C40" t="s">
         <v>657</v>
@@ -7606,23 +7615,40 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>560</v>
+        <v>658</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B41">
+        <v>2.02</v>
+      </c>
+      <c r="C41" t="s">
+        <v>660</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>661</v>
+      </c>
+      <c r="B42">
         <v>2.05</v>
       </c>
-      <c r="C41" t="s">
-        <v>659</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="C42" t="s">
+        <v>662</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
         <v>566</v>
       </c>
     </row>
@@ -7663,19 +7689,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B2">
         <v>2.45</v>
       </c>
       <c r="C2" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>
@@ -7715,19 +7741,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="B2">
         <v>3.18</v>
       </c>
       <c r="C2" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -7767,13 +7793,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="B2">
         <v>0.93</v>
       </c>
       <c r="C2" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -7784,13 +7810,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="B3">
         <v>2.3</v>
       </c>
       <c r="C3" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -7836,19 +7862,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="B2">
         <v>2.17</v>
       </c>
       <c r="C2" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
@@ -7888,19 +7914,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B2">
         <v>3.21</v>
       </c>
       <c r="C2" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -7910,7 +7936,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B322"/>
+  <dimension ref="A1:B323"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7921,12 +7947,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -7934,7 +7960,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -8132,7 +8158,7 @@
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="43" spans="2:2">
@@ -8167,7 +8193,7 @@
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="50" spans="2:2">
@@ -8507,7 +8533,7 @@
     </row>
     <row r="117" spans="2:2">
       <c r="B117" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="118" spans="2:2">
@@ -8672,232 +8698,232 @@
     </row>
     <row r="150" spans="2:2">
       <c r="B150" t="s">
-        <v>272</v>
+        <v>604</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" t="s">
-        <v>604</v>
+        <v>284</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" t="s">
-        <v>286</v>
+        <v>607</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" t="s">
-        <v>670</v>
+        <v>290</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" t="s">
-        <v>292</v>
+        <v>673</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="165" spans="2:2">
       <c r="B165" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="166" spans="2:2">
       <c r="B166" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="167" spans="2:2">
       <c r="B167" t="s">
-        <v>607</v>
+        <v>300</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" t="s">
-        <v>302</v>
+        <v>610</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" t="s">
-        <v>609</v>
+        <v>304</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" t="s">
-        <v>305</v>
+        <v>612</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" t="s">
-        <v>612</v>
+        <v>307</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" t="s">
-        <v>309</v>
+        <v>615</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" t="s">
-        <v>615</v>
+        <v>309</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" t="s">
-        <v>310</v>
+        <v>618</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" t="s">
-        <v>617</v>
+        <v>331</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" t="s">
-        <v>333</v>
+        <v>620</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" t="s">
-        <v>620</v>
+        <v>344</v>
       </c>
     </row>
     <row r="196" spans="2:2">
@@ -8907,82 +8933,82 @@
     </row>
     <row r="197" spans="2:2">
       <c r="B197" t="s">
-        <v>347</v>
+        <v>626</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" t="s">
-        <v>626</v>
+        <v>350</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" t="s">
-        <v>352</v>
+        <v>629</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" t="s">
-        <v>629</v>
+        <v>352</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" t="s">
-        <v>354</v>
+        <v>632</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="206" spans="2:2">
       <c r="B206" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="207" spans="2:2">
       <c r="B207" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="208" spans="2:2">
       <c r="B208" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="209" spans="2:2">
       <c r="B209" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="210" spans="2:2">
       <c r="B210" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="211" spans="2:2">
       <c r="B211" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="212" spans="2:2">
       <c r="B212" t="s">
-        <v>632</v>
+        <v>370</v>
       </c>
     </row>
     <row r="213" spans="2:2">
@@ -8992,407 +9018,407 @@
     </row>
     <row r="214" spans="2:2">
       <c r="B214" t="s">
-        <v>372</v>
+        <v>638</v>
       </c>
     </row>
     <row r="215" spans="2:2">
       <c r="B215" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="216" spans="2:2">
       <c r="B216" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="217" spans="2:2">
       <c r="B217" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="218" spans="2:2">
       <c r="B218" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="219" spans="2:2">
       <c r="B219" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="222" spans="2:2">
       <c r="B222" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="223" spans="2:2">
       <c r="B223" t="s">
-        <v>668</v>
+        <v>390</v>
       </c>
     </row>
     <row r="224" spans="2:2">
       <c r="B224" t="s">
-        <v>391</v>
+        <v>671</v>
       </c>
     </row>
     <row r="225" spans="2:2">
       <c r="B225" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="226" spans="2:2">
       <c r="B226" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="227" spans="2:2">
       <c r="B227" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="228" spans="2:2">
       <c r="B228" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="229" spans="2:2">
       <c r="B229" t="s">
-        <v>638</v>
+        <v>399</v>
       </c>
     </row>
     <row r="230" spans="2:2">
       <c r="B230" t="s">
-        <v>401</v>
+        <v>641</v>
       </c>
     </row>
     <row r="231" spans="2:2">
       <c r="B231" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="232" spans="2:2">
       <c r="B232" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="233" spans="2:2">
       <c r="B233" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="234" spans="2:2">
       <c r="B234" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="235" spans="2:2">
       <c r="B235" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="236" spans="2:2">
       <c r="B236" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="237" spans="2:2">
       <c r="B237" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="238" spans="2:2">
       <c r="B238" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="239" spans="2:2">
       <c r="B239" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="240" spans="2:2">
       <c r="B240" t="s">
-        <v>640</v>
+        <v>420</v>
       </c>
     </row>
     <row r="241" spans="2:2">
       <c r="B241" t="s">
-        <v>422</v>
+        <v>643</v>
       </c>
     </row>
     <row r="242" spans="2:2">
       <c r="B242" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" t="s">
-        <v>643</v>
+        <v>428</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" t="s">
-        <v>430</v>
+        <v>646</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="252" spans="2:2">
       <c r="B252" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="253" spans="2:2">
       <c r="B253" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="257" spans="2:2">
       <c r="B257" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="258" spans="2:2">
       <c r="B258" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="259" spans="2:2">
       <c r="B259" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="260" spans="2:2">
       <c r="B260" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="262" spans="2:2">
       <c r="B262" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="263" spans="2:2">
       <c r="B263" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" t="s">
-        <v>673</v>
+        <v>465</v>
       </c>
     </row>
     <row r="265" spans="2:2">
       <c r="B265" t="s">
-        <v>467</v>
+        <v>676</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" t="s">
-        <v>646</v>
+        <v>467</v>
       </c>
     </row>
     <row r="267" spans="2:2">
       <c r="B267" t="s">
-        <v>469</v>
+        <v>649</v>
       </c>
     </row>
     <row r="268" spans="2:2">
       <c r="B268" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" t="s">
-        <v>649</v>
+        <v>475</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" t="s">
-        <v>477</v>
+        <v>652</v>
       </c>
     </row>
     <row r="273" spans="2:2">
       <c r="B273" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="274" spans="2:2">
       <c r="B274" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="275" spans="2:2">
       <c r="B275" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="276" spans="2:2">
       <c r="B276" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="277" spans="2:2">
       <c r="B277" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="278" spans="2:2">
       <c r="B278" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="279" spans="2:2">
       <c r="B279" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="280" spans="2:2">
       <c r="B280" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="281" spans="2:2">
       <c r="B281" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="285" spans="2:2">
       <c r="B285" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="286" spans="2:2">
       <c r="B286" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="287" spans="2:2">
       <c r="B287" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="288" spans="2:2">
       <c r="B288" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" t="s">
-        <v>651</v>
+        <v>517</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="295" spans="2:2">
@@ -9402,131 +9428,136 @@
     </row>
     <row r="296" spans="2:2">
       <c r="B296" t="s">
-        <v>519</v>
+        <v>659</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" t="s">
-        <v>658</v>
+        <v>531</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" t="s">
-        <v>533</v>
+        <v>661</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="B305" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="B306" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="B307" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="B308" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="B309" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="B310" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="B311" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="B312" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
+      <c r="B313" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
-      <c r="A314" t="s">
-        <v>678</v>
-      </c>
-      <c r="B314" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2">
-      <c r="A316" t="s">
-        <v>679</v>
-      </c>
-      <c r="B316" t="s">
+    <row r="315" spans="1:2">
+      <c r="A315" t="s">
+        <v>681</v>
+      </c>
+      <c r="B315" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
+      <c r="A317" t="s">
+        <v>682</v>
+      </c>
+      <c r="B317" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
-      <c r="B317" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2">
-      <c r="A319" t="s">
-        <v>680</v>
-      </c>
-      <c r="B319" t="s">
+    <row r="318" spans="1:2">
+      <c r="B318" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
+      <c r="A320" t="s">
+        <v>683</v>
+      </c>
+      <c r="B320" t="s">
         <v>579</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2">
-      <c r="B320" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="321" spans="2:2">
       <c r="B321" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="322" spans="2:2">
       <c r="B322" t="s">
-        <v>607</v>
+        <v>598</v>
+      </c>
+    </row>
+    <row r="323" spans="2:2">
+      <c r="B323" t="s">
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weekly update, 2021-12-29, SARS-CoV-2
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
@@ -9,19 +9,20 @@
   <sheets>
     <sheet name="nsp3_Macro1" sheetId="1" r:id="rId1"/>
     <sheet name="nsp3_PL2pro" sheetId="2" r:id="rId2"/>
-    <sheet name="nsp3_NAB" sheetId="3" r:id="rId3"/>
-    <sheet name="nsp3_Ubl2" sheetId="4" r:id="rId4"/>
-    <sheet name="nsp3_pred_linker-Ecto-TM2" sheetId="5" r:id="rId5"/>
-    <sheet name="nsp3_Y3" sheetId="6" r:id="rId6"/>
-    <sheet name="nsp3_Ubl1" sheetId="7" r:id="rId7"/>
-    <sheet name="Organisms" sheetId="8" r:id="rId8"/>
+    <sheet name="nsp3_pred_betaSM" sheetId="3" r:id="rId3"/>
+    <sheet name="nsp3_NAB" sheetId="4" r:id="rId4"/>
+    <sheet name="nsp3_Ubl2" sheetId="5" r:id="rId5"/>
+    <sheet name="nsp3_pred_linker-Ecto-TM2" sheetId="6" r:id="rId6"/>
+    <sheet name="nsp3_Y3" sheetId="7" r:id="rId7"/>
+    <sheet name="nsp3_Ubl1" sheetId="8" r:id="rId8"/>
+    <sheet name="Organisms" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1619" uniqueCount="690">
   <si>
     <t>PDB</t>
   </si>
@@ -2019,6 +2020,15 @@
   </si>
   <si>
     <t>THE CRYSTAL STRUCTURE OF PAPAIN-LIKE PROTEASE OF SARS COV-2 , C111S MUTANT, IN COMPLEX WITH PLP_SNYDER530 INHIBITOR</t>
+  </si>
+  <si>
+    <t>7t9w</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE NSP3 BSM (BETACORONAVIRUS-SPECIFIC MARKER) DOMAIN FROM SARS-COV-2</t>
+  </si>
+  <si>
+    <t>2021-12-20</t>
   </si>
   <si>
     <t>7lgo</t>
@@ -7718,7 +7728,7 @@
         <v>666</v>
       </c>
       <c r="B2">
-        <v>2.45</v>
+        <v>2.2</v>
       </c>
       <c r="C2" t="s">
         <v>667</v>
@@ -7770,7 +7780,7 @@
         <v>669</v>
       </c>
       <c r="B2">
-        <v>3.18</v>
+        <v>2.45</v>
       </c>
       <c r="C2" t="s">
         <v>670</v>
@@ -7788,6 +7798,58 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>672</v>
+      </c>
+      <c r="B2">
+        <v>3.18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>673</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -7819,13 +7881,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="B2">
         <v>0.93</v>
       </c>
       <c r="C2" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -7836,71 +7898,19 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="B3">
         <v>2.3</v>
       </c>
       <c r="C3" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>569</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="110.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>676</v>
-      </c>
-      <c r="B2">
-        <v>2.17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>677</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -7943,7 +7953,7 @@
         <v>679</v>
       </c>
       <c r="B2">
-        <v>3.21</v>
+        <v>2.17</v>
       </c>
       <c r="C2" t="s">
         <v>680</v>
@@ -7952,7 +7962,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>617</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -7962,7 +7972,59 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B324"/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>682</v>
+      </c>
+      <c r="B2">
+        <v>3.21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B325"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7973,12 +8035,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -7986,7 +8048,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -8149,1445 +8211,1450 @@
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>68</v>
+        <v>666</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" t="s">
-        <v>570</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>80</v>
+        <v>570</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" t="s">
-        <v>666</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" t="s">
-        <v>83</v>
+        <v>669</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>669</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" t="s">
-        <v>95</v>
+        <v>672</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" t="s">
-        <v>573</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" t="s">
-        <v>99</v>
+        <v>573</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" t="s">
-        <v>576</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" t="s">
-        <v>125</v>
+        <v>576</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" t="s">
-        <v>579</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" t="s">
-        <v>131</v>
+        <v>579</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" t="s">
-        <v>582</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" t="s">
-        <v>137</v>
+        <v>582</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84" t="s">
-        <v>585</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" t="s">
-        <v>154</v>
+        <v>585</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" t="s">
-        <v>588</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92" t="s">
-        <v>166</v>
+        <v>588</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95" t="s">
-        <v>591</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96" t="s">
-        <v>172</v>
+        <v>591</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="108" spans="2:2">
       <c r="B108" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="109" spans="2:2">
       <c r="B109" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="2:2">
       <c r="B111" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="113" spans="2:2">
       <c r="B113" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" spans="2:2">
       <c r="B118" t="s">
-        <v>672</v>
+        <v>217</v>
       </c>
     </row>
     <row r="119" spans="2:2">
       <c r="B119" t="s">
-        <v>593</v>
+        <v>675</v>
       </c>
     </row>
     <row r="120" spans="2:2">
       <c r="B120" t="s">
-        <v>219</v>
+        <v>593</v>
       </c>
     </row>
     <row r="121" spans="2:2">
       <c r="B121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="123" spans="2:2">
       <c r="B123" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="125" spans="2:2">
       <c r="B125" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" spans="2:2">
       <c r="B126" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="128" spans="2:2">
       <c r="B128" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" t="s">
-        <v>596</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="2:2">
       <c r="B130" t="s">
-        <v>238</v>
+        <v>596</v>
       </c>
     </row>
     <row r="131" spans="2:2">
       <c r="B131" t="s">
-        <v>598</v>
+        <v>238</v>
       </c>
     </row>
     <row r="132" spans="2:2">
       <c r="B132" t="s">
-        <v>240</v>
+        <v>598</v>
       </c>
     </row>
     <row r="133" spans="2:2">
       <c r="B133" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" t="s">
-        <v>601</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" t="s">
-        <v>250</v>
+        <v>601</v>
       </c>
     </row>
     <row r="138" spans="2:2">
       <c r="B138" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" t="s">
-        <v>603</v>
+        <v>252</v>
       </c>
     </row>
     <row r="140" spans="2:2">
       <c r="B140" t="s">
-        <v>254</v>
+        <v>603</v>
       </c>
     </row>
     <row r="141" spans="2:2">
       <c r="B141" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="142" spans="2:2">
       <c r="B142" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="143" spans="2:2">
       <c r="B143" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="144" spans="2:2">
       <c r="B144" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="145" spans="2:2">
       <c r="B145" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="147" spans="2:2">
       <c r="B147" t="s">
-        <v>605</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" t="s">
-        <v>269</v>
+        <v>605</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" t="s">
-        <v>607</v>
+        <v>273</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" t="s">
-        <v>275</v>
+        <v>607</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" t="s">
-        <v>610</v>
+        <v>287</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" t="s">
-        <v>289</v>
+        <v>610</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" t="s">
-        <v>676</v>
+        <v>293</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" t="s">
-        <v>295</v>
+        <v>679</v>
       </c>
     </row>
     <row r="165" spans="2:2">
       <c r="B165" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="166" spans="2:2">
       <c r="B166" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="167" spans="2:2">
       <c r="B167" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" t="s">
-        <v>613</v>
+        <v>303</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" t="s">
-        <v>305</v>
+        <v>613</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" t="s">
-        <v>615</v>
+        <v>307</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" t="s">
-        <v>308</v>
+        <v>615</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" t="s">
-        <v>618</v>
+        <v>310</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" t="s">
-        <v>312</v>
+        <v>618</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" t="s">
-        <v>621</v>
+        <v>312</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" t="s">
-        <v>313</v>
+        <v>621</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" t="s">
-        <v>623</v>
+        <v>334</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" t="s">
-        <v>336</v>
+        <v>623</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="197" spans="2:2">
       <c r="B197" t="s">
-        <v>626</v>
+        <v>347</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" t="s">
-        <v>350</v>
+        <v>629</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" t="s">
-        <v>632</v>
+        <v>353</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" t="s">
-        <v>355</v>
+        <v>632</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" t="s">
-        <v>635</v>
+        <v>355</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" t="s">
-        <v>357</v>
+        <v>635</v>
       </c>
     </row>
     <row r="206" spans="2:2">
       <c r="B206" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="207" spans="2:2">
       <c r="B207" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="208" spans="2:2">
       <c r="B208" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="209" spans="2:2">
       <c r="B209" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="210" spans="2:2">
       <c r="B210" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="211" spans="2:2">
       <c r="B211" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="212" spans="2:2">
       <c r="B212" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="213" spans="2:2">
       <c r="B213" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="214" spans="2:2">
       <c r="B214" t="s">
-        <v>638</v>
+        <v>373</v>
       </c>
     </row>
     <row r="215" spans="2:2">
       <c r="B215" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="216" spans="2:2">
       <c r="B216" t="s">
-        <v>375</v>
+        <v>641</v>
       </c>
     </row>
     <row r="217" spans="2:2">
       <c r="B217" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="218" spans="2:2">
       <c r="B218" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="219" spans="2:2">
       <c r="B219" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="222" spans="2:2">
       <c r="B222" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="223" spans="2:2">
       <c r="B223" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="224" spans="2:2">
       <c r="B224" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="225" spans="2:2">
       <c r="B225" t="s">
-        <v>674</v>
+        <v>393</v>
       </c>
     </row>
     <row r="226" spans="2:2">
       <c r="B226" t="s">
-        <v>394</v>
+        <v>677</v>
       </c>
     </row>
     <row r="227" spans="2:2">
       <c r="B227" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="228" spans="2:2">
       <c r="B228" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="229" spans="2:2">
       <c r="B229" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="230" spans="2:2">
       <c r="B230" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="231" spans="2:2">
       <c r="B231" t="s">
-        <v>644</v>
+        <v>402</v>
       </c>
     </row>
     <row r="232" spans="2:2">
       <c r="B232" t="s">
-        <v>404</v>
+        <v>644</v>
       </c>
     </row>
     <row r="233" spans="2:2">
       <c r="B233" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="234" spans="2:2">
       <c r="B234" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="235" spans="2:2">
       <c r="B235" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="236" spans="2:2">
       <c r="B236" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="237" spans="2:2">
       <c r="B237" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="238" spans="2:2">
       <c r="B238" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="239" spans="2:2">
       <c r="B239" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="240" spans="2:2">
       <c r="B240" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="241" spans="2:2">
       <c r="B241" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="242" spans="2:2">
       <c r="B242" t="s">
-        <v>646</v>
+        <v>423</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" t="s">
-        <v>425</v>
+        <v>646</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" t="s">
-        <v>649</v>
+        <v>431</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" t="s">
-        <v>433</v>
+        <v>649</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="252" spans="2:2">
       <c r="B252" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="253" spans="2:2">
       <c r="B253" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="257" spans="2:2">
       <c r="B257" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="258" spans="2:2">
       <c r="B258" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="259" spans="2:2">
       <c r="B259" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="260" spans="2:2">
       <c r="B260" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="262" spans="2:2">
       <c r="B262" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="263" spans="2:2">
       <c r="B263" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="265" spans="2:2">
       <c r="B265" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" t="s">
-        <v>679</v>
+        <v>468</v>
       </c>
     </row>
     <row r="267" spans="2:2">
       <c r="B267" t="s">
-        <v>470</v>
+        <v>682</v>
       </c>
     </row>
     <row r="268" spans="2:2">
       <c r="B268" t="s">
-        <v>652</v>
+        <v>470</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" t="s">
-        <v>472</v>
+        <v>652</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="273" spans="2:2">
       <c r="B273" t="s">
-        <v>655</v>
+        <v>478</v>
       </c>
     </row>
     <row r="274" spans="2:2">
       <c r="B274" t="s">
-        <v>480</v>
+        <v>655</v>
       </c>
     </row>
     <row r="275" spans="2:2">
       <c r="B275" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="276" spans="2:2">
       <c r="B276" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="277" spans="2:2">
       <c r="B277" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="278" spans="2:2">
       <c r="B278" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="279" spans="2:2">
       <c r="B279" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="280" spans="2:2">
       <c r="B280" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="281" spans="2:2">
       <c r="B281" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="285" spans="2:2">
       <c r="B285" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="286" spans="2:2">
       <c r="B286" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="287" spans="2:2">
       <c r="B287" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="288" spans="2:2">
       <c r="B288" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" t="s">
-        <v>657</v>
+        <v>520</v>
       </c>
     </row>
     <row r="296" spans="2:2">
       <c r="B296" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" t="s">
-        <v>522</v>
+        <v>662</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="B305" t="s">
-        <v>664</v>
+        <v>534</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="B306" t="s">
-        <v>536</v>
+        <v>664</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="B307" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="B308" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="B309" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="B310" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="B311" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="B312" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="B313" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="B314" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2">
+      <c r="B315" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
-      <c r="A316" t="s">
-        <v>684</v>
-      </c>
-      <c r="B316" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2">
-      <c r="A318" t="s">
-        <v>685</v>
-      </c>
-      <c r="B318" t="s">
+    <row r="317" spans="1:2">
+      <c r="A317" t="s">
+        <v>687</v>
+      </c>
+      <c r="B317" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="A319" t="s">
+        <v>688</v>
+      </c>
+      <c r="B319" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
-      <c r="B319" t="s">
+    <row r="320" spans="1:2">
+      <c r="B320" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
-      <c r="A321" t="s">
-        <v>686</v>
-      </c>
-      <c r="B321" t="s">
+    <row r="322" spans="1:2">
+      <c r="A322" t="s">
+        <v>689</v>
+      </c>
+      <c r="B322" t="s">
         <v>582</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2">
-      <c r="B322" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="323" spans="1:2">
       <c r="B323" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
     </row>
     <row r="324" spans="1:2">
       <c r="B324" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="B325" t="s">
         <v>613</v>
       </c>
     </row>

</xml_diff>

<commit_message>
weekly update 2022-01-19, SARS-CoV-2
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
@@ -7,24 +7,25 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="domain1" sheetId="1" r:id="rId1"/>
-    <sheet name="domain2" sheetId="2" r:id="rId2"/>
-    <sheet name="domain3" sheetId="3" r:id="rId3"/>
-    <sheet name="domain4" sheetId="4" r:id="rId4"/>
-    <sheet name="domain5" sheetId="5" r:id="rId5"/>
-    <sheet name="domain6" sheetId="6" r:id="rId6"/>
-    <sheet name="domain7" sheetId="7" r:id="rId7"/>
-    <sheet name="domain8" sheetId="8" r:id="rId8"/>
-    <sheet name="domain9" sheetId="9" r:id="rId9"/>
-    <sheet name="domain10" sheetId="10" r:id="rId10"/>
-    <sheet name="Organisms" sheetId="11" r:id="rId11"/>
+    <sheet name="nsp3_Macro1_" sheetId="1" r:id="rId1"/>
+    <sheet name="nsp3_Ubl2_nsp3_PL2pro_" sheetId="2" r:id="rId2"/>
+    <sheet name="nsp3_Ubl2_" sheetId="3" r:id="rId3"/>
+    <sheet name="nsp3_betaSM-M_" sheetId="4" r:id="rId4"/>
+    <sheet name="nsp3_DPUP_nsp3_Ubl2_" sheetId="5" r:id="rId5"/>
+    <sheet name="nsp3_NAB_" sheetId="6" r:id="rId6"/>
+    <sheet name="nsp3_PL2pro_" sheetId="7" r:id="rId7"/>
+    <sheet name="nsp3_Macro1_nsp3_PL2pro_" sheetId="8" r:id="rId8"/>
+    <sheet name="nsp3_Y3_" sheetId="9" r:id="rId9"/>
+    <sheet name="None" sheetId="10" r:id="rId10"/>
+    <sheet name="nsp3_Ubl1_" sheetId="11" r:id="rId11"/>
+    <sheet name="Organisms" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="704">
   <si>
     <t>nsp3_Macro1_</t>
   </si>
@@ -2007,6 +2008,18 @@
   </si>
   <si>
     <t>2021-12-20</t>
+  </si>
+  <si>
+    <t>nsp3_DPUP_nsp3_Ubl2_</t>
+  </si>
+  <si>
+    <t>7thh</t>
+  </si>
+  <si>
+    <t>SUD-C AND UBL2 DOMAINS OF SARS COV-2 NSP3 PROTEIN</t>
+  </si>
+  <si>
+    <t>2022-01-11</t>
   </si>
   <si>
     <t>nsp3_NAB_</t>
@@ -7038,7 +7051,7 @@
         <v>692</v>
       </c>
       <c r="B3">
-        <v>3.21</v>
+        <v>2.72</v>
       </c>
       <c r="C3" t="s">
         <v>693</v>
@@ -7047,7 +7060,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>604</v>
+        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -7057,7 +7070,64 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B325"/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>696</v>
+      </c>
+      <c r="B3">
+        <v>3.21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>697</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>604</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B326"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7068,12 +7138,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -7081,7 +7151,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -7269,1425 +7339,1430 @@
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>77</v>
+        <v>662</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>649</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" t="s">
-        <v>81</v>
+        <v>649</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" t="s">
-        <v>662</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" t="s">
-        <v>84</v>
+        <v>666</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" t="s">
-        <v>652</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>96</v>
+        <v>652</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" t="s">
-        <v>666</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" t="s">
-        <v>100</v>
+        <v>670</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" t="s">
-        <v>569</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" t="s">
-        <v>126</v>
+        <v>569</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" t="s">
-        <v>572</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>132</v>
+        <v>572</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" t="s">
-        <v>575</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" t="s">
-        <v>138</v>
+        <v>575</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" t="s">
-        <v>578</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" t="s">
-        <v>155</v>
+        <v>578</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92" t="s">
-        <v>581</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93" t="s">
-        <v>167</v>
+        <v>581</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96" t="s">
-        <v>669</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" t="s">
-        <v>173</v>
+        <v>673</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="108" spans="2:2">
       <c r="B108" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="109" spans="2:2">
       <c r="B109" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="111" spans="2:2">
       <c r="B111" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="113" spans="2:2">
       <c r="B113" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="118" spans="2:2">
       <c r="B118" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="119" spans="2:2">
       <c r="B119" t="s">
-        <v>681</v>
+        <v>218</v>
       </c>
     </row>
     <row r="120" spans="2:2">
       <c r="B120" t="s">
-        <v>671</v>
+        <v>685</v>
       </c>
     </row>
     <row r="121" spans="2:2">
       <c r="B121" t="s">
-        <v>220</v>
+        <v>675</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="2:2">
       <c r="B123" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="125" spans="2:2">
       <c r="B125" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="126" spans="2:2">
       <c r="B126" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="128" spans="2:2">
       <c r="B128" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="130" spans="2:2">
       <c r="B130" t="s">
-        <v>584</v>
+        <v>237</v>
       </c>
     </row>
     <row r="131" spans="2:2">
       <c r="B131" t="s">
-        <v>239</v>
+        <v>584</v>
       </c>
     </row>
     <row r="132" spans="2:2">
       <c r="B132" t="s">
-        <v>586</v>
+        <v>239</v>
       </c>
     </row>
     <row r="133" spans="2:2">
       <c r="B133" t="s">
-        <v>241</v>
+        <v>586</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" t="s">
-        <v>589</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="2:2">
       <c r="B138" t="s">
-        <v>251</v>
+        <v>589</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="140" spans="2:2">
       <c r="B140" t="s">
-        <v>673</v>
+        <v>253</v>
       </c>
     </row>
     <row r="141" spans="2:2">
       <c r="B141" t="s">
-        <v>255</v>
+        <v>677</v>
       </c>
     </row>
     <row r="142" spans="2:2">
       <c r="B142" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="143" spans="2:2">
       <c r="B143" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="144" spans="2:2">
       <c r="B144" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="145" spans="2:2">
       <c r="B145" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="147" spans="2:2">
       <c r="B147" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" t="s">
-        <v>592</v>
+        <v>268</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" t="s">
-        <v>270</v>
+        <v>592</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" t="s">
-        <v>594</v>
+        <v>274</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" t="s">
-        <v>276</v>
+        <v>594</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" t="s">
-        <v>597</v>
+        <v>288</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" t="s">
-        <v>290</v>
+        <v>597</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" t="s">
-        <v>684</v>
+        <v>294</v>
       </c>
     </row>
     <row r="165" spans="2:2">
       <c r="B165" t="s">
-        <v>296</v>
+        <v>688</v>
       </c>
     </row>
     <row r="166" spans="2:2">
       <c r="B166" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="167" spans="2:2">
       <c r="B167" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" t="s">
-        <v>600</v>
+        <v>304</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" t="s">
-        <v>306</v>
+        <v>600</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" t="s">
-        <v>602</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" t="s">
-        <v>309</v>
+        <v>602</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" t="s">
-        <v>605</v>
+        <v>311</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" t="s">
-        <v>313</v>
+        <v>605</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" t="s">
-        <v>608</v>
+        <v>313</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" t="s">
-        <v>314</v>
+        <v>608</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" t="s">
-        <v>610</v>
+        <v>335</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" t="s">
-        <v>337</v>
+        <v>610</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="197" spans="2:2">
       <c r="B197" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" t="s">
-        <v>613</v>
+        <v>348</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" t="s">
-        <v>351</v>
+        <v>616</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" t="s">
-        <v>675</v>
+        <v>354</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" t="s">
-        <v>356</v>
+        <v>679</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" t="s">
-        <v>688</v>
+        <v>356</v>
       </c>
     </row>
     <row r="206" spans="2:2">
       <c r="B206" t="s">
-        <v>358</v>
+        <v>692</v>
       </c>
     </row>
     <row r="207" spans="2:2">
       <c r="B207" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="208" spans="2:2">
       <c r="B208" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="209" spans="2:2">
       <c r="B209" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="210" spans="2:2">
       <c r="B210" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="211" spans="2:2">
       <c r="B211" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="212" spans="2:2">
       <c r="B212" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="213" spans="2:2">
       <c r="B213" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="214" spans="2:2">
       <c r="B214" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="215" spans="2:2">
       <c r="B215" t="s">
-        <v>619</v>
+        <v>374</v>
       </c>
     </row>
     <row r="216" spans="2:2">
       <c r="B216" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="217" spans="2:2">
       <c r="B217" t="s">
-        <v>376</v>
+        <v>622</v>
       </c>
     </row>
     <row r="218" spans="2:2">
       <c r="B218" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="219" spans="2:2">
       <c r="B219" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="222" spans="2:2">
       <c r="B222" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="223" spans="2:2">
       <c r="B223" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="224" spans="2:2">
       <c r="B224" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="225" spans="2:2">
       <c r="B225" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="226" spans="2:2">
       <c r="B226" t="s">
-        <v>625</v>
+        <v>394</v>
       </c>
     </row>
     <row r="227" spans="2:2">
       <c r="B227" t="s">
-        <v>395</v>
+        <v>625</v>
       </c>
     </row>
     <row r="228" spans="2:2">
       <c r="B228" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="229" spans="2:2">
       <c r="B229" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="230" spans="2:2">
       <c r="B230" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="231" spans="2:2">
       <c r="B231" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="232" spans="2:2">
       <c r="B232" t="s">
-        <v>627</v>
+        <v>403</v>
       </c>
     </row>
     <row r="233" spans="2:2">
       <c r="B233" t="s">
-        <v>405</v>
+        <v>627</v>
       </c>
     </row>
     <row r="234" spans="2:2">
       <c r="B234" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="235" spans="2:2">
       <c r="B235" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="236" spans="2:2">
       <c r="B236" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="237" spans="2:2">
       <c r="B237" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="238" spans="2:2">
       <c r="B238" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="239" spans="2:2">
       <c r="B239" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="240" spans="2:2">
       <c r="B240" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="241" spans="2:2">
       <c r="B241" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="242" spans="2:2">
       <c r="B242" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" t="s">
-        <v>629</v>
+        <v>424</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" t="s">
-        <v>426</v>
+        <v>629</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" t="s">
-        <v>632</v>
+        <v>432</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" t="s">
-        <v>434</v>
+        <v>632</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="252" spans="2:2">
       <c r="B252" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="253" spans="2:2">
       <c r="B253" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="257" spans="2:2">
       <c r="B257" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="258" spans="2:2">
       <c r="B258" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="259" spans="2:2">
       <c r="B259" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="260" spans="2:2">
       <c r="B260" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="262" spans="2:2">
       <c r="B262" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="263" spans="2:2">
       <c r="B263" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="265" spans="2:2">
       <c r="B265" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="267" spans="2:2">
       <c r="B267" t="s">
-        <v>692</v>
+        <v>469</v>
       </c>
     </row>
     <row r="268" spans="2:2">
       <c r="B268" t="s">
-        <v>471</v>
+        <v>696</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" t="s">
-        <v>635</v>
+        <v>471</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" t="s">
-        <v>473</v>
+        <v>635</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="273" spans="2:2">
       <c r="B273" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="274" spans="2:2">
       <c r="B274" t="s">
-        <v>655</v>
+        <v>479</v>
       </c>
     </row>
     <row r="275" spans="2:2">
       <c r="B275" t="s">
-        <v>481</v>
+        <v>655</v>
       </c>
     </row>
     <row r="276" spans="2:2">
       <c r="B276" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="277" spans="2:2">
       <c r="B277" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="278" spans="2:2">
       <c r="B278" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="279" spans="2:2">
       <c r="B279" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="280" spans="2:2">
       <c r="B280" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="281" spans="2:2">
       <c r="B281" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="285" spans="2:2">
       <c r="B285" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="286" spans="2:2">
       <c r="B286" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="287" spans="2:2">
       <c r="B287" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="288" spans="2:2">
       <c r="B288" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="296" spans="2:2">
       <c r="B296" t="s">
-        <v>638</v>
+        <v>521</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" t="s">
-        <v>523</v>
+        <v>643</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="B305" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="B306" t="s">
-        <v>678</v>
+        <v>535</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="B307" t="s">
-        <v>537</v>
+        <v>682</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="B308" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="B309" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="B310" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="B311" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="B312" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="B313" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="B314" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="315" spans="1:2">
       <c r="B315" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2">
+      <c r="B316" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
-      <c r="A317" t="s">
-        <v>697</v>
-      </c>
-      <c r="B317" t="s">
+    <row r="318" spans="1:2">
+      <c r="A318" t="s">
+        <v>701</v>
+      </c>
+      <c r="B318" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
-      <c r="A319" t="s">
-        <v>698</v>
-      </c>
-      <c r="B319" t="s">
+    <row r="320" spans="1:2">
+      <c r="A320" t="s">
+        <v>702</v>
+      </c>
+      <c r="B320" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
-      <c r="B320" t="s">
+    <row r="321" spans="1:2">
+      <c r="B321" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
-      <c r="A322" t="s">
-        <v>699</v>
-      </c>
-      <c r="B322" t="s">
+    <row r="323" spans="1:2">
+      <c r="A323" t="s">
+        <v>703</v>
+      </c>
+      <c r="B323" t="s">
         <v>575</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2">
-      <c r="B323" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="324" spans="1:2">
       <c r="B324" t="s">
-        <v>589</v>
+        <v>675</v>
       </c>
     </row>
     <row r="325" spans="1:2">
       <c r="B325" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="B326" t="s">
         <v>600</v>
       </c>
     </row>
@@ -9485,7 +9560,7 @@
         <v>662</v>
       </c>
       <c r="B3">
-        <v>2.45</v>
+        <v>1.32</v>
       </c>
       <c r="C3" t="s">
         <v>663</v>
@@ -9503,6 +9578,63 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>666</v>
+      </c>
+      <c r="B3">
+        <v>2.45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>667</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -9517,7 +9649,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9539,47 +9671,47 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="B3">
         <v>1.9</v>
       </c>
       <c r="C3" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="B4">
         <v>2.11</v>
       </c>
       <c r="C4" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="B5">
         <v>2.7</v>
       </c>
       <c r="C5" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -9590,13 +9722,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="B6">
         <v>2.58</v>
       </c>
       <c r="C6" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -9607,93 +9739,36 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="B7">
         <v>1.93</v>
       </c>
       <c r="C7" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="B8">
         <v>2.05</v>
       </c>
       <c r="C8" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
         <v>568</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="110.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>681</v>
-      </c>
-      <c r="B3">
-        <v>0.93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>682</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -9716,7 +9791,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9738,19 +9813,19 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B3">
-        <v>2.17</v>
+        <v>0.93</v>
       </c>
       <c r="C3" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>686</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -9798,7 +9873,7 @@
         <v>688</v>
       </c>
       <c r="B3">
-        <v>2.72</v>
+        <v>2.17</v>
       </c>
       <c r="C3" t="s">
         <v>689</v>

</xml_diff>

<commit_message>
weekly update, 2022-01-26, SARS-CoV-2
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="707">
   <si>
     <t>nsp3_Macro1_</t>
   </si>
@@ -2119,6 +2119,15 @@
   </si>
   <si>
     <t>CRYSTAL STRUCTURE OF THE UBIQUITIN-LIKE DOMAIN 1 (UBL1) OF NSP3 FROM SARS-COV-2</t>
+  </si>
+  <si>
+    <t>7ti9</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF THE UBIQUITIN-LIKE DOMAIN 1 (UBL1) OF NSP3 FROM SARS-COV-2, FORM 2</t>
+  </si>
+  <si>
+    <t>2022-01-13</t>
   </si>
   <si>
     <t>Lists all PDBs which contain sequences of a certain organism.</t>
@@ -7070,7 +7079,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7120,6 +7129,23 @@
         <v>604</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>698</v>
+      </c>
+      <c r="B4">
+        <v>2.73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>699</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>700</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7127,7 +7153,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B326"/>
+  <dimension ref="A1:B327"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7138,12 +7164,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -7151,7 +7177,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -8489,280 +8515,285 @@
     </row>
     <row r="270" spans="2:2">
       <c r="B270" t="s">
-        <v>635</v>
+        <v>698</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" t="s">
-        <v>473</v>
+        <v>635</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="273" spans="2:2">
       <c r="B273" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="274" spans="2:2">
       <c r="B274" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="275" spans="2:2">
       <c r="B275" t="s">
-        <v>655</v>
+        <v>479</v>
       </c>
     </row>
     <row r="276" spans="2:2">
       <c r="B276" t="s">
-        <v>481</v>
+        <v>655</v>
       </c>
     </row>
     <row r="277" spans="2:2">
       <c r="B277" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="278" spans="2:2">
       <c r="B278" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="279" spans="2:2">
       <c r="B279" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="280" spans="2:2">
       <c r="B280" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="281" spans="2:2">
       <c r="B281" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="285" spans="2:2">
       <c r="B285" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="286" spans="2:2">
       <c r="B286" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="287" spans="2:2">
       <c r="B287" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="288" spans="2:2">
       <c r="B288" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="296" spans="2:2">
       <c r="B296" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" t="s">
-        <v>638</v>
+        <v>521</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" t="s">
-        <v>523</v>
+        <v>643</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="B305" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="B306" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="B307" t="s">
-        <v>682</v>
+        <v>535</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="B308" t="s">
-        <v>537</v>
+        <v>682</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="B309" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="B310" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="B311" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="B312" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="B313" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="B314" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="315" spans="1:2">
       <c r="B315" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="316" spans="1:2">
       <c r="B316" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
+      <c r="B317" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
-      <c r="A318" t="s">
-        <v>701</v>
-      </c>
-      <c r="B318" t="s">
+    <row r="319" spans="1:2">
+      <c r="A319" t="s">
+        <v>704</v>
+      </c>
+      <c r="B319" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
-      <c r="A320" t="s">
-        <v>702</v>
-      </c>
-      <c r="B320" t="s">
+    <row r="321" spans="1:2">
+      <c r="A321" t="s">
+        <v>705</v>
+      </c>
+      <c r="B321" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
-      <c r="B321" t="s">
+    <row r="322" spans="1:2">
+      <c r="B322" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
-      <c r="A323" t="s">
-        <v>703</v>
-      </c>
-      <c r="B323" t="s">
+    <row r="324" spans="1:2">
+      <c r="A324" t="s">
+        <v>706</v>
+      </c>
+      <c r="B324" t="s">
         <v>575</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2">
-      <c r="B324" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="325" spans="1:2">
       <c r="B325" t="s">
-        <v>589</v>
+        <v>675</v>
       </c>
     </row>
     <row r="326" spans="1:2">
       <c r="B326" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="B327" t="s">
         <v>600</v>
       </c>
     </row>

</xml_diff>

<commit_message>
weekly update, 2022-02-02, SARS-CoV-2
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV-2/domains_and_infos_of_nsp3.xlsx
@@ -17,15 +17,16 @@
     <sheet name="nsp3_Macro1_nsp3_PL2pro_" sheetId="8" r:id="rId8"/>
     <sheet name="nsp3_Y3_" sheetId="9" r:id="rId9"/>
     <sheet name="None" sheetId="10" r:id="rId10"/>
-    <sheet name="nsp3_Ubl1_" sheetId="11" r:id="rId11"/>
-    <sheet name="Organisms" sheetId="12" r:id="rId12"/>
+    <sheet name="nsp3_PL2pro_nsp3_Ubl2_" sheetId="11" r:id="rId11"/>
+    <sheet name="nsp3_Ubl1_" sheetId="12" r:id="rId12"/>
+    <sheet name="Organisms" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="711">
   <si>
     <t>nsp3_Macro1_</t>
   </si>
@@ -2110,6 +2111,18 @@
   </si>
   <si>
     <t>2020-11-20</t>
+  </si>
+  <si>
+    <t>nsp3_PL2pro_nsp3_Ubl2_</t>
+  </si>
+  <si>
+    <t>7nt4</t>
+  </si>
+  <si>
+    <t>X-RAY STRUCTURE OF SCOV2-PLPRO IN COMPLEX WITH SMALL MOLECULE INHIBITOR</t>
+  </si>
+  <si>
+    <t>2021-03-09</t>
   </si>
   <si>
     <t>nsp3_Ubl1_</t>
@@ -7079,6 +7092,63 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>696</v>
+      </c>
+      <c r="B3">
+        <v>2.68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>697</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>698</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7092,7 +7162,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -7114,13 +7184,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="B3">
         <v>3.21</v>
       </c>
       <c r="C3" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -7131,19 +7201,19 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="B4">
         <v>2.73</v>
       </c>
       <c r="C4" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -7151,9 +7221,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B327"/>
+  <dimension ref="A1:B328"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7164,12 +7234,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -7177,7 +7247,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -8510,290 +8580,295 @@
     </row>
     <row r="269" spans="2:2">
       <c r="B269" t="s">
-        <v>471</v>
+        <v>700</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" t="s">
-        <v>698</v>
+        <v>471</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" t="s">
-        <v>635</v>
+        <v>702</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" t="s">
-        <v>473</v>
+        <v>635</v>
       </c>
     </row>
     <row r="273" spans="2:2">
       <c r="B273" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="274" spans="2:2">
       <c r="B274" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="275" spans="2:2">
       <c r="B275" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="276" spans="2:2">
       <c r="B276" t="s">
-        <v>655</v>
+        <v>479</v>
       </c>
     </row>
     <row r="277" spans="2:2">
       <c r="B277" t="s">
-        <v>481</v>
+        <v>655</v>
       </c>
     </row>
     <row r="278" spans="2:2">
       <c r="B278" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="279" spans="2:2">
       <c r="B279" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="280" spans="2:2">
       <c r="B280" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="281" spans="2:2">
       <c r="B281" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="285" spans="2:2">
       <c r="B285" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="286" spans="2:2">
       <c r="B286" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="287" spans="2:2">
       <c r="B287" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="288" spans="2:2">
       <c r="B288" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="296" spans="2:2">
       <c r="B296" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" t="s">
-        <v>638</v>
+        <v>521</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" t="s">
-        <v>523</v>
+        <v>643</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="B305" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="B306" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="B307" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="B308" t="s">
-        <v>682</v>
+        <v>535</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="B309" t="s">
-        <v>537</v>
+        <v>682</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="B310" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="B311" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="B312" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="B313" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="B314" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="315" spans="1:2">
       <c r="B315" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="316" spans="1:2">
       <c r="B316" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="317" spans="1:2">
       <c r="B317" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
+      <c r="B318" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
-      <c r="A319" t="s">
-        <v>704</v>
-      </c>
-      <c r="B319" t="s">
+    <row r="320" spans="1:2">
+      <c r="A320" t="s">
+        <v>708</v>
+      </c>
+      <c r="B320" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
-      <c r="A321" t="s">
-        <v>705</v>
-      </c>
-      <c r="B321" t="s">
+    <row r="322" spans="1:2">
+      <c r="A322" t="s">
+        <v>709</v>
+      </c>
+      <c r="B322" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
-      <c r="B322" t="s">
+    <row r="323" spans="1:2">
+      <c r="B323" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
-      <c r="A324" t="s">
-        <v>706</v>
-      </c>
-      <c r="B324" t="s">
+    <row r="325" spans="1:2">
+      <c r="A325" t="s">
+        <v>710</v>
+      </c>
+      <c r="B325" t="s">
         <v>575</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2">
-      <c r="B325" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="326" spans="1:2">
       <c r="B326" t="s">
-        <v>589</v>
+        <v>675</v>
       </c>
     </row>
     <row r="327" spans="1:2">
       <c r="B327" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="B328" t="s">
         <v>600</v>
       </c>
     </row>

</xml_diff>